<commit_message>
feat: Add Geo Trades Service monitor tool and unify terminology
</commit_message>
<xml_diff>
--- a/Data/Monitor-SCFI-Trends.xlsx
+++ b/Data/Monitor-SCFI-Trends.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29608"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Applications\Cursor\Shipping Schedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Applications\Cursor\Shipping Schedule\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA2E016-F7B1-4400-BC6C-DDF799E5A8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BCCBDF-DCC9-4202-A53C-D033314FBD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIN Timeseries - W" sheetId="2" r:id="rId1"/>
@@ -532,13 +532,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S810"/>
+  <dimension ref="A1:S811"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B764" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A810" sqref="A810"/>
+      <selection pane="bottomRight" activeCell="A811" sqref="A811"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -43293,53 +43293,106 @@
       <c r="A810" s="9">
         <v>45996</v>
       </c>
-      <c r="B810" s="11">
+      <c r="B810" s="10">
         <v>1397.63</v>
       </c>
-      <c r="C810" s="11">
+      <c r="C810" s="10">
         <v>1276</v>
       </c>
-      <c r="D810" s="11">
+      <c r="D810" s="10">
         <v>321</v>
       </c>
-      <c r="E810" s="11">
+      <c r="E810" s="10">
         <v>2214</v>
       </c>
-      <c r="F810" s="11">
+      <c r="F810" s="10">
         <v>2315</v>
       </c>
-      <c r="G810" s="11">
+      <c r="G810" s="10">
         <v>1400</v>
       </c>
-      <c r="H810" s="11">
+      <c r="H810" s="10">
         <v>143</v>
       </c>
-      <c r="I810" s="11">
+      <c r="I810" s="10">
         <v>2300</v>
       </c>
-      <c r="J810" s="11">
+      <c r="J810" s="10">
         <v>1781</v>
       </c>
-      <c r="K810" s="11">
+      <c r="K810" s="10">
         <v>2222</v>
       </c>
-      <c r="L810" s="11">
+      <c r="L810" s="10">
         <v>1689</v>
       </c>
-      <c r="M810" s="11">
+      <c r="M810" s="10">
         <v>543</v>
       </c>
-      <c r="N810" s="11">
+      <c r="N810" s="10">
         <v>3457</v>
       </c>
-      <c r="O810" s="11">
+      <c r="O810" s="10">
         <v>312</v>
       </c>
-      <c r="P810" s="11">
+      <c r="P810" s="10">
         <v>1550</v>
       </c>
-      <c r="Q810" s="11">
+      <c r="Q810" s="10">
         <v>1604</v>
+      </c>
+    </row>
+    <row r="811" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A811" s="6">
+        <v>46003</v>
+      </c>
+      <c r="B811" s="11">
+        <v>1506.46</v>
+      </c>
+      <c r="C811" s="11">
+        <v>1241</v>
+      </c>
+      <c r="D811" s="11">
+        <v>321</v>
+      </c>
+      <c r="E811" s="11">
+        <v>2112</v>
+      </c>
+      <c r="F811" s="11">
+        <v>2652</v>
+      </c>
+      <c r="G811" s="11">
+        <v>1538</v>
+      </c>
+      <c r="H811" s="11">
+        <v>139</v>
+      </c>
+      <c r="I811" s="11">
+        <v>2737</v>
+      </c>
+      <c r="J811" s="11">
+        <v>1881</v>
+      </c>
+      <c r="K811" s="11">
+        <v>2218</v>
+      </c>
+      <c r="L811" s="11">
+        <v>1486</v>
+      </c>
+      <c r="M811" s="11">
+        <v>556</v>
+      </c>
+      <c r="N811" s="11">
+        <v>3393</v>
+      </c>
+      <c r="O811" s="11">
+        <v>312</v>
+      </c>
+      <c r="P811" s="11">
+        <v>1780</v>
+      </c>
+      <c r="Q811" s="11">
+        <v>1388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Release v1.6.6: Add user access control, auto-load data files, fix week calculation, and enhance access log tooltips
</commit_message>
<xml_diff>
--- a/Data/Monitor-SCFI-Trends.xlsx
+++ b/Data/Monitor-SCFI-Trends.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29615"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Applications\Cursor\Shipping Schedule\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Applications\Cursor\Shipping Schedule\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCD4E74-EB65-41BC-A606-F06D2E069924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E595B925-216D-4597-8F15-6929D48FBBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIN Timeseries - W" sheetId="2" r:id="rId1"/>
@@ -203,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,6 +225,9 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -529,13 +532,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S811"/>
+  <dimension ref="A1:S812"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B764" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A812" sqref="A812"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -43392,6 +43395,59 @@
         <v>1388</v>
       </c>
     </row>
+    <row r="812" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A812" s="9">
+        <v>46010</v>
+      </c>
+      <c r="B812" s="11">
+        <v>1552.92</v>
+      </c>
+      <c r="C812" s="11">
+        <v>1263</v>
+      </c>
+      <c r="D812" s="11">
+        <v>321</v>
+      </c>
+      <c r="E812" s="11">
+        <v>2125</v>
+      </c>
+      <c r="F812" s="11">
+        <v>2846</v>
+      </c>
+      <c r="G812" s="11">
+        <v>1533</v>
+      </c>
+      <c r="H812" s="11">
+        <v>138</v>
+      </c>
+      <c r="I812" s="11">
+        <v>2833</v>
+      </c>
+      <c r="J812" s="11">
+        <v>2015</v>
+      </c>
+      <c r="K812" s="11">
+        <v>2212</v>
+      </c>
+      <c r="L812" s="11">
+        <v>1291</v>
+      </c>
+      <c r="M812" s="11">
+        <v>542</v>
+      </c>
+      <c r="N812" s="11">
+        <v>3238</v>
+      </c>
+      <c r="O812" s="11">
+        <v>312</v>
+      </c>
+      <c r="P812" s="11">
+        <v>1992</v>
+      </c>
+      <c r="Q812" s="11">
+        <v>1294</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Release v2.0.0: Major updates and improvements
- Added user authentication system with Gist-based whitelist
- Implemented port sorting utilities with unified sorting logic
- Added 001-03 and 365-03 port standardizer tools
- Enhanced multi-select functionality for port filters
- Improved Excel file reading with week sheet parsing
- Updated dashboard and sidebar navigation
- Fixed port sorting issues (e.g., Indonesia-Philippines region)
- Added Admin tools (Workouts, Access Log)
- Updated Monitor tools with manual file loading
- Code quality improvements: removed duplicates, unified utilities
- Fixed data/index.json configuration files
</commit_message>
<xml_diff>
--- a/Data/Monitor-SCFI-Trends.xlsx
+++ b/Data/Monitor-SCFI-Trends.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29617"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Applications\Cursor\Shipping Schedule\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E595B925-216D-4597-8F15-6929D48FBBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C29AC9-ECAB-40E0-A3A0-12DBDBAF6A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIN Timeseries - W" sheetId="2" r:id="rId1"/>
@@ -532,13 +532,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S812"/>
+  <dimension ref="A1:S813"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B764" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A812" sqref="A812"/>
+      <selection pane="bottomRight" activeCell="A813" sqref="A813"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -43399,53 +43399,106 @@
       <c r="A812" s="9">
         <v>46010</v>
       </c>
-      <c r="B812" s="11">
+      <c r="B812" s="10">
         <v>1552.92</v>
       </c>
-      <c r="C812" s="11">
+      <c r="C812" s="10">
         <v>1263</v>
       </c>
-      <c r="D812" s="11">
+      <c r="D812" s="10">
         <v>321</v>
       </c>
-      <c r="E812" s="11">
+      <c r="E812" s="10">
         <v>2125</v>
       </c>
-      <c r="F812" s="11">
+      <c r="F812" s="10">
         <v>2846</v>
       </c>
-      <c r="G812" s="11">
+      <c r="G812" s="10">
         <v>1533</v>
       </c>
-      <c r="H812" s="11">
+      <c r="H812" s="10">
         <v>138</v>
       </c>
-      <c r="I812" s="11">
+      <c r="I812" s="10">
         <v>2833</v>
       </c>
-      <c r="J812" s="11">
+      <c r="J812" s="10">
         <v>2015</v>
       </c>
-      <c r="K812" s="11">
+      <c r="K812" s="10">
         <v>2212</v>
       </c>
-      <c r="L812" s="11">
+      <c r="L812" s="10">
         <v>1291</v>
       </c>
-      <c r="M812" s="11">
+      <c r="M812" s="10">
         <v>542</v>
       </c>
-      <c r="N812" s="11">
+      <c r="N812" s="10">
         <v>3238</v>
       </c>
-      <c r="O812" s="11">
+      <c r="O812" s="10">
         <v>312</v>
       </c>
-      <c r="P812" s="11">
+      <c r="P812" s="10">
         <v>1992</v>
       </c>
-      <c r="Q812" s="11">
+      <c r="Q812" s="10">
         <v>1294</v>
+      </c>
+    </row>
+    <row r="813" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A813" s="6">
+        <v>46017</v>
+      </c>
+      <c r="B813" s="11">
+        <v>1656.32</v>
+      </c>
+      <c r="C813" s="11">
+        <v>1346</v>
+      </c>
+      <c r="D813" s="11">
+        <v>321</v>
+      </c>
+      <c r="E813" s="11">
+        <v>2182</v>
+      </c>
+      <c r="F813" s="11">
+        <v>3033</v>
+      </c>
+      <c r="G813" s="11">
+        <v>1690</v>
+      </c>
+      <c r="H813" s="11">
+        <v>142</v>
+      </c>
+      <c r="I813" s="11">
+        <v>3143</v>
+      </c>
+      <c r="J813" s="11">
+        <v>2120</v>
+      </c>
+      <c r="K813" s="11">
+        <v>2356</v>
+      </c>
+      <c r="L813" s="11">
+        <v>1292</v>
+      </c>
+      <c r="M813" s="11">
+        <v>548</v>
+      </c>
+      <c r="N813" s="11">
+        <v>3201</v>
+      </c>
+      <c r="O813" s="11">
+        <v>312</v>
+      </c>
+      <c r="P813" s="11">
+        <v>2188</v>
+      </c>
+      <c r="Q813" s="11">
+        <v>1266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>